<commit_message>
Actualizacion de la memoria
</commit_message>
<xml_diff>
--- a/06. Manuales/Memoria_ema.xlsx
+++ b/06. Manuales/Memoria_ema.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Iteraciones" sheetId="1" r:id="rId1"/>
     <sheet name="Calendario" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -169,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>fase</t>
   </si>
@@ -387,6 +388,12 @@
   </si>
   <si>
     <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>FASE INICIO</t>
+  </si>
+  <si>
+    <t>ITERACION N°1</t>
   </si>
 </sst>
 </file>
@@ -1079,14 +1086,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1104,21 +1105,12 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1127,59 +1119,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1191,6 +1135,69 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1543,7 +1550,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="51" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="5">
@@ -1576,7 +1583,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="51"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -1589,7 +1596,7 @@
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="4"/>
@@ -1605,7 +1612,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -1620,7 +1627,7 @@
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1638,7 +1645,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="52"/>
       <c r="B5">
         <v>2</v>
       </c>
@@ -1785,7 +1792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -1795,575 +1802,575 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15">
+      <c r="C3" s="21"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13">
         <v>1</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="13">
         <v>2</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="13">
         <v>3</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="13">
         <v>4</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="14">
         <v>5</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="26">
+      <c r="A4" s="31"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="22">
         <v>6</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>7</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>8</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <v>9</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="12">
         <v>10</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="12">
         <v>11</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="15">
         <v>12</v>
       </c>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="26">
+      <c r="A5" s="31"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="22">
         <v>13</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>14</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>15</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>16</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="12">
         <v>17</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>18</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="15">
         <v>19</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="26">
+      <c r="A6" s="31"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="22">
         <v>20</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>21</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="26">
         <v>22</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <v>23</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <v>24</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>25</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="15">
         <v>26</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32">
+      <c r="A7" s="31"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="27">
         <v>27</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="28">
         <v>28</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="29">
         <v>29</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="30">
         <v>30</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="26">
         <v>31</v>
       </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="48" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="15">
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="13">
         <v>1</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="14">
         <v>2</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="26">
+      <c r="A9" s="31"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="22">
         <v>3</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>4</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="12">
         <v>5</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="26">
         <v>6</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="12">
         <v>7</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>8</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="15">
         <v>9</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="52">
+      <c r="A10" s="31"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="36">
         <v>10</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>11</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="28">
         <v>12</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="24">
         <v>13</v>
       </c>
-      <c r="G10" s="62">
+      <c r="G10" s="41">
         <v>14</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="12">
         <v>15</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="15">
         <v>16</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="26">
+      <c r="A11" s="31"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="22">
         <v>17</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="42">
         <v>18</v>
       </c>
-      <c r="E11" s="66">
+      <c r="E11" s="45">
         <v>19</v>
       </c>
-      <c r="F11" s="64">
+      <c r="F11" s="43">
         <v>20</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <v>21</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="12">
         <v>22</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="15">
         <v>23</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="27">
+      <c r="A12" s="31"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="23">
         <v>24</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>25</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="44">
         <v>26</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <v>27</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <v>28</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="16">
         <v>29</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="17">
         <v>30</v>
       </c>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="43" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="13">
         <v>1</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="46">
         <v>2</v>
       </c>
-      <c r="E13" s="66">
+      <c r="E13" s="45">
         <v>3</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="47">
         <v>4</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="13">
         <v>5</v>
       </c>
-      <c r="H13" s="70">
+      <c r="H13" s="49">
         <v>6</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="14">
         <v>7</v>
       </c>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="14">
+      <c r="A14" s="31"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="12">
         <v>8</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <v>9</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="35">
         <v>10</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="33">
         <v>11</v>
       </c>
-      <c r="G14" s="61">
+      <c r="G14" s="40">
         <v>12</v>
       </c>
-      <c r="H14" s="71">
+      <c r="H14" s="50">
         <v>13</v>
       </c>
-      <c r="I14" s="69">
+      <c r="I14" s="48">
         <v>14</v>
       </c>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="14">
+      <c r="A15" s="31"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="12">
         <v>15</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>16</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>17</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="12">
         <v>18</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="12">
         <v>19</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="35">
         <v>20</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="15">
         <v>21</v>
       </c>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="14">
+      <c r="A16" s="31"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="12">
         <v>22</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="12">
         <v>23</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="26">
         <v>24</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="12">
         <v>25</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="34">
         <v>26</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="12">
         <v>27</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="15">
         <v>28</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="18">
+      <c r="A17" s="31"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="16">
         <v>29</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="25">
         <v>30</v>
       </c>
-      <c r="E17" s="71">
+      <c r="E17" s="50">
         <v>31</v>
       </c>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="58" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="15">
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="13">
         <v>1</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="13">
         <v>2</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="13">
         <v>3</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="14">
         <v>4</v>
       </c>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="14">
+      <c r="A19" s="32"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="12">
         <v>5</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="26">
         <v>6</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="26">
         <v>7</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="12">
         <v>8</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="12">
         <v>9</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="12">
         <v>10</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="15">
         <v>11</v>
       </c>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="61">
+      <c r="A20" s="32"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="40">
         <v>12</v>
       </c>
-      <c r="D20" s="71">
+      <c r="D20" s="50">
         <v>13</v>
       </c>
-      <c r="E20" s="71">
+      <c r="E20" s="50">
         <v>14</v>
       </c>
-      <c r="F20" s="62">
+      <c r="F20" s="41">
         <v>15</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="26">
         <v>16</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="12">
         <v>17</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="15">
         <v>18</v>
       </c>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="14">
+      <c r="A21" s="32"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="12">
         <v>19</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="35">
         <v>20</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="35">
         <v>21</v>
       </c>
-      <c r="F21" s="61">
+      <c r="F21" s="40">
         <v>22</v>
       </c>
-      <c r="G21" s="71">
+      <c r="G21" s="50">
         <v>23</v>
       </c>
-      <c r="H21" s="62">
+      <c r="H21" s="41">
         <v>24</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="15">
         <v>25</v>
       </c>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="18">
+      <c r="A22" s="32"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="16">
         <v>26</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="16">
         <v>27</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="16">
         <v>28</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <v>29</v>
       </c>
-      <c r="G22" s="65">
+      <c r="G22" s="44">
         <v>30</v>
       </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
+      <c r="A23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
+      <c r="A24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
+      <c r="A25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2378,4 +2385,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>